<commit_message>
tabla semaforo: add bg colors to all vbles
</commit_message>
<xml_diff>
--- a/datos/indicadores_umbrales.xlsx
+++ b/datos/indicadores_umbrales.xlsx
@@ -193,11 +193,11 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -254,7 +254,7 @@
         <v>0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="I2" s="2" t="n">
         <v>0</v>
@@ -286,7 +286,7 @@
         <v>4</v>
       </c>
       <c r="H3" s="2" t="n">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="I3" s="2" t="n">
         <v>2</v>
@@ -318,7 +318,7 @@
         <v>7</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="I4" s="2" t="n">
         <v>5</v>
@@ -350,7 +350,7 @@
         <v>10</v>
       </c>
       <c r="H5" s="2" t="n">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2" t="n">
         <v>10</v>
@@ -381,8 +381,8 @@
       <c r="G6" s="2" t="n">
         <v>15</v>
       </c>
-      <c r="H6" s="2" t="n">
-        <v>30</v>
+      <c r="H6" s="0" t="n">
+        <v>0</v>
       </c>
       <c r="I6" s="2" t="n">
         <v>15</v>

</xml_diff>